<commit_message>
Dimension s hinzugefügt, funktioniert zu 80%
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>17000</v>
+        <v>9800</v>
       </c>
       <c r="C2" t="n">
-        <v>4000</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Der Entscheidungsvariable a den Skill hinzugef.
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="C2" t="n">
-        <v>800</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Änderungen an Nebenbedingungen vorgenommen
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1800</v>
+        <v>12900</v>
       </c>
       <c r="C2" t="n">
-        <v>800</v>
+        <v>-9100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NB13 eingebaut + Allg. Anpassungen vorgenommen
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>12900</v>
+        <v>14600</v>
       </c>
       <c r="C2" t="n">
-        <v>-9100</v>
+        <v>-7400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Timetable Daten speichern am ändern
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2</f>
+              <f>'Kosten'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2</f>
+              <f>'Kosten'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2</f>
+              <f>'Kosten'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2</f>
+              <f>'Kosten'!$C$2:$C$3</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,9 +621,20 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
+        <v>13900</v>
+      </c>
+      <c r="C2" t="n">
         <v>13100</v>
       </c>
-      <c r="C2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>13100</v>
+      </c>
+      <c r="C3" t="n">
         <v>13100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Timetable Daten in der Db korrekt speichern
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$3</f>
+              <f>'Kosten'!$A$2:$A$14</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2:$B$3</f>
+              <f>'Kosten'!$B$2:$B$14</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$3</f>
+              <f>'Kosten'!$A$2:$A$14</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2:$C$3</f>
+              <f>'Kosten'!$C$2:$C$14</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>13900</v>
+        <v>28600</v>
       </c>
       <c r="C2" t="n">
-        <v>13100</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="3">
@@ -632,10 +632,131 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>13100</v>
+        <v>25000</v>
       </c>
       <c r="C3" t="n">
-        <v>13100</v>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>24300</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B5" t="n">
+        <v>24000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B6" t="n">
+        <v>24000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
+        <v>24000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>35</v>
+      </c>
+      <c r="B8" t="n">
+        <v>24000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>40</v>
+      </c>
+      <c r="B9" t="n">
+        <v>24000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>23800</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>23800</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>23800</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>23800</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>23800</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prints gelöscht, kleine Anpassungen
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>19250</v>
+        <v>17150</v>
       </c>
       <c r="C2" t="n">
         <v>15150</v>
@@ -632,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>16450</v>
+        <v>16650</v>
       </c>
       <c r="C3" t="n">
         <v>15150</v>
@@ -643,7 +643,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>15850</v>
+        <v>15950</v>
       </c>
       <c r="C4" t="n">
         <v>15150</v>
@@ -654,7 +654,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>15850</v>
+        <v>15950</v>
       </c>
       <c r="C5" t="n">
         <v>15150</v>

</xml_diff>

<commit_message>
id aus timetable gelöscht (save data in database)
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$6</f>
+              <f>'Kosten'!$A$2:$A$14</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2:$B$6</f>
+              <f>'Kosten'!$B$2:$B$14</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$6</f>
+              <f>'Kosten'!$A$2:$A$14</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2:$C$6</f>
+              <f>'Kosten'!$C$2:$C$14</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>17150</v>
+        <v>33850</v>
       </c>
       <c r="C2" t="n">
         <v>15150</v>
@@ -632,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>16650</v>
+        <v>30250</v>
       </c>
       <c r="C3" t="n">
         <v>15150</v>
@@ -643,7 +643,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>15950</v>
+        <v>28950</v>
       </c>
       <c r="C4" t="n">
         <v>15150</v>
@@ -654,7 +654,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>15950</v>
+        <v>26950</v>
       </c>
       <c r="C5" t="n">
         <v>15150</v>
@@ -665,9 +665,97 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
+        <v>25950</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
+        <v>24450</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>35</v>
+      </c>
+      <c r="B8" t="n">
+        <v>16350</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>40</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15850</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>15850</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>15850</v>
+      </c>
+      <c r="C11" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>15850</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>15850</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
         <v>15750</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C14" t="n">
         <v>15150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NB13 + NB15 angepasst
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$14</f>
+              <f>'Kosten'!$A$2</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2:$B$14</f>
+              <f>'Kosten'!$B$2</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$14</f>
+              <f>'Kosten'!$A$2</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2:$C$14</f>
+              <f>'Kosten'!$C$2</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,141 +621,9 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>33850</v>
+        <v>53550</v>
       </c>
       <c r="C2" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" t="n">
-        <v>30250</v>
-      </c>
-      <c r="C3" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>15</v>
-      </c>
-      <c r="B4" t="n">
-        <v>28950</v>
-      </c>
-      <c r="C4" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>20</v>
-      </c>
-      <c r="B5" t="n">
-        <v>26950</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B6" t="n">
-        <v>25950</v>
-      </c>
-      <c r="C6" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>30</v>
-      </c>
-      <c r="B7" t="n">
-        <v>24450</v>
-      </c>
-      <c r="C7" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>35</v>
-      </c>
-      <c r="B8" t="n">
-        <v>16350</v>
-      </c>
-      <c r="C8" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>40</v>
-      </c>
-      <c r="B9" t="n">
-        <v>15850</v>
-      </c>
-      <c r="C9" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>45</v>
-      </c>
-      <c r="B10" t="n">
-        <v>15850</v>
-      </c>
-      <c r="C10" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>50</v>
-      </c>
-      <c r="B11" t="n">
-        <v>15850</v>
-      </c>
-      <c r="C11" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>55</v>
-      </c>
-      <c r="B12" t="n">
-        <v>15850</v>
-      </c>
-      <c r="C12" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>60</v>
-      </c>
-      <c r="B13" t="n">
-        <v>15850</v>
-      </c>
-      <c r="C13" t="n">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>65</v>
-      </c>
-      <c r="B14" t="n">
-        <v>15750</v>
-      </c>
-      <c r="C14" t="n">
         <v>15150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NB14 erweitert + excel_output start und end_time2
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2</f>
+              <f>'Kosten'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2</f>
+              <f>'Kosten'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2</f>
+              <f>'Kosten'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2</f>
+              <f>'Kosten'!$C$2:$C$3</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,10 +621,21 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>53550</v>
+        <v>25350</v>
       </c>
       <c r="C2" t="n">
-        <v>15150</v>
+        <v>14950</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>14950</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vorüberprüfung 1 und 2 umgebaut + getestet
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$9</f>
+              <f>'Kosten'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2:$B$9</f>
+              <f>'Kosten'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$9</f>
+              <f>'Kosten'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2:$C$9</f>
+              <f>'Kosten'!$C$2:$C$7</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>31250</v>
+        <v>29550</v>
       </c>
       <c r="C3" t="n">
         <v>14950</v>
@@ -643,7 +643,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>30450</v>
+        <v>27850</v>
       </c>
       <c r="C4" t="n">
         <v>14950</v>
@@ -654,7 +654,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>29150</v>
+        <v>24850</v>
       </c>
       <c r="C5" t="n">
         <v>14950</v>
@@ -665,7 +665,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>22100</v>
+        <v>22750</v>
       </c>
       <c r="C6" t="n">
         <v>14950</v>
@@ -676,31 +676,9 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>15950</v>
+        <v>15150</v>
       </c>
       <c r="C7" t="n">
-        <v>14950</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>35</v>
-      </c>
-      <c r="B8" t="n">
-        <v>15550</v>
-      </c>
-      <c r="C8" t="n">
-        <v>14950</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>40</v>
-      </c>
-      <c r="B9" t="n">
-        <v>15150</v>
-      </c>
-      <c r="C9" t="n">
         <v>14950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiple changes: new week selection, compl solver
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>21500</v>
+        <v>2450</v>
       </c>
       <c r="C2" t="n">
-        <v>6500</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
massive change on session logic
</commit_message>
<xml_diff>
--- a/Kostenanalyse.xlsx
+++ b/Kostenanalyse.xlsx
@@ -169,12 +169,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$7</f>
+              <f>'Kosten'!$A$2:$A$30</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$B$2:$B$7</f>
+              <f>'Kosten'!$B$2:$B$30</f>
             </numRef>
           </val>
         </ser>
@@ -201,12 +201,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Kosten'!$A$2:$A$7</f>
+              <f>'Kosten'!$A$2:$A$30</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kosten'!$C$2:$C$7</f>
+              <f>'Kosten'!$C$2:$C$30</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>61214</v>
+        <v>35850</v>
       </c>
       <c r="C2" t="n">
-        <v>17350</v>
+        <v>15100</v>
       </c>
     </row>
     <row r="3">
@@ -632,10 +632,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>33416</v>
+        <v>35850</v>
       </c>
       <c r="C3" t="n">
-        <v>17350</v>
+        <v>15100</v>
       </c>
     </row>
     <row r="4">
@@ -643,10 +643,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>18758</v>
+        <v>35850</v>
       </c>
       <c r="C4" t="n">
-        <v>17350</v>
+        <v>15100</v>
       </c>
     </row>
     <row r="5">
@@ -654,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>18758</v>
+        <v>35850</v>
       </c>
       <c r="C5" t="n">
-        <v>17350</v>
+        <v>15100</v>
       </c>
     </row>
     <row r="6">
@@ -665,10 +665,10 @@
         <v>25</v>
       </c>
       <c r="B6" t="n">
-        <v>18758</v>
+        <v>35850</v>
       </c>
       <c r="C6" t="n">
-        <v>17350</v>
+        <v>15100</v>
       </c>
     </row>
     <row r="7">
@@ -676,10 +676,263 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>17359</v>
+        <v>35850</v>
       </c>
       <c r="C7" t="n">
-        <v>17350</v>
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>35</v>
+      </c>
+      <c r="B8" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>40</v>
+      </c>
+      <c r="B9" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C11" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C14" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C15" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="B17" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+      <c r="B18" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C18" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>90</v>
+      </c>
+      <c r="B19" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>95</v>
+      </c>
+      <c r="B20" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C20" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C21" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>105</v>
+      </c>
+      <c r="B22" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C22" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>110</v>
+      </c>
+      <c r="B23" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C23" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>115</v>
+      </c>
+      <c r="B24" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C24" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>120</v>
+      </c>
+      <c r="B25" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C25" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125</v>
+      </c>
+      <c r="B26" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>130</v>
+      </c>
+      <c r="B27" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C27" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>135</v>
+      </c>
+      <c r="B28" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C28" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>140</v>
+      </c>
+      <c r="B29" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C29" t="n">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>145</v>
+      </c>
+      <c r="B30" t="n">
+        <v>35850</v>
+      </c>
+      <c r="C30" t="n">
+        <v>15100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>